<commit_message>
added lecture 12 and section 12. 11 missing(thanksgiving break)
</commit_message>
<xml_diff>
--- a/Homework/LateDays.xlsx
+++ b/Homework/LateDays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khan_\Downloads\cs82_advanced_machine_learning_git\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4548856-B60A-4615-B382-53299A0ACAE7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC958189-D0CB-4E02-813B-55FE85889C04}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25230" windowHeight="11445" xr2:uid="{92E6A1DF-06BB-456F-9032-1B13E06544C1}"/>
   </bookViews>
@@ -67,8 +67,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,8 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E827A7EE-5CBC-4E0D-8020-AF483EA03C6A}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +512,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <f>SUM(B1:B10)</f>
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>